<commit_message>
Cleaning up temp files
</commit_message>
<xml_diff>
--- a/Clustering/Per file ion set data.xlsx
+++ b/Clustering/Per file ion set data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jeffreyvanhumbeck/Documents/GitHub/Bitumen-ML/Clustering/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3AA8C28D-6F7F-9D41-8D9A-BC16DEFA2500}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AF94867-EE45-3D48-A47D-8F4D89243BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6920" yWindow="800" windowWidth="21800" windowHeight="15820" xr2:uid="{73E943CB-B167-C842-9FE7-42C1AA4FB68E}"/>
+    <workbookView xWindow="6920" yWindow="1540" windowWidth="21800" windowHeight="15820" xr2:uid="{73E943CB-B167-C842-9FE7-42C1AA4FB68E}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>File Name</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>% Zero</t>
+  </si>
+  <si>
+    <t>Pairwise Relationships</t>
   </si>
 </sst>
 </file>
@@ -421,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE0CF3A9-5695-4246-A454-D2F76364754E}">
-  <dimension ref="A1:E41"/>
+  <dimension ref="A1:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E41" sqref="E41"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,9 +435,10 @@
     <col min="2" max="2" width="26" customWidth="1"/>
     <col min="3" max="3" width="32.5" customWidth="1"/>
     <col min="4" max="4" width="26" customWidth="1"/>
+    <col min="6" max="6" width="21.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -450,8 +454,11 @@
       <c r="E1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>19208</v>
       </c>
@@ -470,7 +477,7 @@
         <v>48.903938691855288</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>19209</v>
       </c>
@@ -489,7 +496,7 @@
         <v>50.796050876100686</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>19210</v>
       </c>
@@ -508,7 +515,7 @@
         <v>45.420460632029993</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>19211</v>
       </c>
@@ -527,7 +534,7 @@
         <v>57.745474003388921</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>19212</v>
       </c>
@@ -546,7 +553,7 @@
         <v>40.194503925767307</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>19213</v>
       </c>
@@ -565,7 +572,7 @@
         <v>43.606878731177048</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>19214</v>
       </c>
@@ -584,7 +591,7 @@
         <v>43.746105225674356</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>19215</v>
       </c>
@@ -603,7 +610,7 @@
         <v>42.010515996791732</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>19216</v>
       </c>
@@ -622,7 +629,7 @@
         <v>41.350891337454087</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>19217</v>
       </c>
@@ -641,7 +648,7 @@
         <v>43.012671782973406</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>19218</v>
       </c>
@@ -660,7 +667,7 @@
         <v>45.348630380647457</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>19219</v>
       </c>
@@ -679,7 +686,7 @@
         <v>40.019630588025343</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>19220</v>
       </c>
@@ -698,7 +705,7 @@
         <v>42.364268520994919</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>19221</v>
       </c>
@@ -717,7 +724,7 @@
         <v>41.86274509803922</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>19222</v>
       </c>

</xml_diff>